<commit_message>
Internal data from single source file
</commit_message>
<xml_diff>
--- a/data-raw/Suporte.xlsx
+++ b/data-raw/Suporte.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="CBO" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5267" uniqueCount="4997">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5267" uniqueCount="4999">
   <si>
     <t>Oficial General da Aeronautica</t>
   </si>
@@ -15012,22 +15012,28 @@
     <t>Outras Atividades de Serviços Pessoais não Especificadas Anteriormente</t>
   </si>
   <si>
-    <t>cbo</t>
-  </si>
-  <si>
     <t>cnae_secao</t>
   </si>
   <si>
-    <t>cnae_grupo</t>
-  </si>
-  <si>
     <t>cnae_divisao</t>
   </si>
   <si>
-    <t>cnae_classe</t>
-  </si>
-  <si>
-    <t>cnae_subclasse</t>
+    <t>nomes_cbo</t>
+  </si>
+  <si>
+    <t>nomes_cnae_secao</t>
+  </si>
+  <si>
+    <t>nomes_cnae_divisao</t>
+  </si>
+  <si>
+    <t>nomes_cnae_grupo</t>
+  </si>
+  <si>
+    <t>nomes_cnae_classe</t>
+  </si>
+  <si>
+    <t>nomes_cnae_subclasse</t>
   </si>
 </sst>
 </file>
@@ -15406,7 +15412,7 @@
         <v>2718</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4991</v>
+        <v>4993</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -37163,7 +37169,7 @@
   <dimension ref="A1:B88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37174,10 +37180,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4994</v>
+        <v>4992</v>
       </c>
       <c r="B1" t="s">
-        <v>4992</v>
+        <v>4991</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -37885,8 +37891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37896,7 +37902,7 @@
         <v>2718</v>
       </c>
       <c r="B1" t="s">
-        <v>4992</v>
+        <v>4994</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -38085,7 +38091,7 @@
   <dimension ref="A1:B88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38095,7 +38101,7 @@
         <v>2718</v>
       </c>
       <c r="B1" t="s">
-        <v>4994</v>
+        <v>4995</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -38804,7 +38810,7 @@
   <dimension ref="A1:B287"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38814,7 +38820,7 @@
         <v>2718</v>
       </c>
       <c r="B1" t="s">
-        <v>4993</v>
+        <v>4996</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -41114,8 +41120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B675"/>
   <sheetViews>
-    <sheetView topLeftCell="A637" workbookViewId="0">
-      <selection activeCell="A675" sqref="A675"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41125,7 +41131,7 @@
         <v>2718</v>
       </c>
       <c r="B1" t="s">
-        <v>4995</v>
+        <v>4997</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -46529,8 +46535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1358"/>
   <sheetViews>
-    <sheetView topLeftCell="A1320" workbookViewId="0">
-      <selection activeCell="F1325" sqref="F1325"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46540,7 +46546,7 @@
         <v>2718</v>
       </c>
       <c r="B1" t="s">
-        <v>4996</v>
+        <v>4998</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -57405,21 +57411,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100AB78960618B7BE469D38D7868DD16947" ma:contentTypeVersion="8" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="3f4cbbd60fbc4a5b22483f9625f8b189">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ee36cee3-c53f-4c35-9944-9258ac9d330b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d45ae86d0ec39606f18fafbaf432c8c8" ns2:_="">
     <xsd:import namespace="ee36cee3-c53f-4c35-9944-9258ac9d330b"/>
@@ -57589,24 +57580,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDDCFDDC-586B-4E62-ABFF-27975DB0BC0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2BA774A-A8E4-43CC-854A-1C4D7C8881A6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E2E427C-1EE0-458A-AD86-B0A8B0A5FDDD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -57622,4 +57611,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2BA774A-A8E4-43CC-854A-1C4D7C8881A6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDDCFDDC-586B-4E62-ABFF-27975DB0BC0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>